<commit_message>
Descriptions of functions, inifinity for loop, debuger
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>SNIPETS</t>
   </si>
@@ -51,6 +51,30 @@
   </si>
   <si>
     <t>foreach + twice tab = foreach(var item in collection)</t>
+  </si>
+  <si>
+    <t>Progress in training</t>
+  </si>
+  <si>
+    <t>Wstęp</t>
+  </si>
+  <si>
+    <t>Start application with parameters (ppm on project &gt; properties &gt; debug &gt; start options)</t>
+  </si>
+  <si>
+    <t>if + twice tab = if (true) { }</t>
+  </si>
+  <si>
+    <t>eslse + twice tab = else { }</t>
+  </si>
+  <si>
+    <t>Pętla nie kończąca się for ( ; ; ) { }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Szybkie generowanie metod ppm na zaznaczone linijku kodu &gt; quick actions… &gt; extract method </t>
+  </si>
+  <si>
+    <t>/// summary opis</t>
   </si>
 </sst>
 </file>
@@ -65,12 +89,36 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -85,8 +133,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -367,31 +419,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.44140625" customWidth="1"/>
-    <col min="2" max="2" width="58.33203125" customWidth="1"/>
-    <col min="3" max="3" width="40.109375" customWidth="1"/>
+    <col min="2" max="2" width="82.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -401,8 +457,11 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -411,6 +470,32 @@
       </c>
       <c r="C3" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
exceptions, writing to txt END OF PART I
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>SNIPETS</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>eslse + twice tab = else { }</t>
-  </si>
-  <si>
-    <t>Pętla nie kończąca się for ( ; ; ) { }</t>
   </si>
   <si>
     <t xml:space="preserve">Szybkie generowanie metod ppm na zaznaczone linijku kodu &gt; quick actions… &gt; extract method </t>
@@ -208,16 +205,412 @@
   </si>
   <si>
     <t>Delegat - zmienna która odwołuje się do metody a nie obiektu jakies klasy czy też zmiennej wartosciowej. Delegaty mają zmienne które wskazują na metody</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Skrócony IF. Condition ? True : false ; przykład: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">int malo = lol == "chuj" ? a = 2 : a = 3; </t>
+    </r>
+  </si>
+  <si>
+    <t>Konstrukucję SWITCH używamy często jako alternatywy dla if else</t>
+  </si>
+  <si>
+    <t>sw + twice tab</t>
+  </si>
+  <si>
+    <r>
+      <t>for (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>inicjalizacja</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>warunek</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>inkrementacja</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)
+            {
+               wykonywane instrukcje
+            }</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>while (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>warunek</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">)
+            {
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                 PĘTLA WHILE SPRAWDZA WARUNEK NA POCZĄTKU!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+            }</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">do
+{
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>PĘTLA  DO WHILE SPRAWDZA WARUNEK NA KOŃCU!. KOD WYKONA SIĘ NA PEWNO 1 RAZ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+} while (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>warunek</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">foreach (var item in collection)
+{
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>PĘTLA TA ZAWSZE WYKONUJE SIĘ NA JAKIMŚ ZBIORZE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+}</t>
+    </r>
+  </si>
+  <si>
+    <t>Pętla nie kończąca się for ( ; ; ) { } oraz while (true) to też pętla nieskończona</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>break</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - wychodzi z pętli, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>continue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - przechodzi do następnej iteracji pomijając kod, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>goto</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - przechodzenie do innego kodu w tej samej metodzie - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>nie powinno goto się używać bo zaciemnia kod</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">return - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>wychodzenie z metody</t>
+    </r>
+  </si>
+  <si>
+    <t>Obsługa wyjątków jest bezpieczna. Rzucamy obiektami.</t>
+  </si>
+  <si>
+    <t>ctrl + k + d = wyrównywanie kodu</t>
+  </si>
+  <si>
+    <t>stos to są metody wywowływane po sobie np.: main --&gt; method1 --&gt; method2 itd.</t>
+  </si>
+  <si>
+    <t>Jeżeli nikt nie będzie subskrybował zadarzeń to event będzie nullem i będzie zglaszal null reference exception</t>
+  </si>
+  <si>
+    <t>Obsłużenie wyjątku powoduje ze program się nie zawiesza. Wyjątki obsługujemy od najbardziej szczegółowych do najmniej szczegółowych.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>finally</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> będzie zawsze wykonywany, nawet kiedy nie zaistnieje wyjątek w bloku kodu try</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>using</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> to to samo co </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>try</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">finally. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Trzeba zwalniac zasoby po skorzystaniu z nich. Np. zamykać plik tekstowy jak się wyciągnie z niego dane.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="4"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -562,10 +955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -592,10 +985,10 @@
         <v>9</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -612,7 +1005,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -640,214 +1033,290 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="B47" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="B48" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="B49" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="B50" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B51" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" s="6" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>